<commit_message>
fixed to Excel  table and rendering of DT in HTML
</commit_message>
<xml_diff>
--- a/edit_docs/data/lists_2022-05-03.xlsx
+++ b/edit_docs/data/lists_2022-05-03.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{A030CF20-61C1-4EC1-9CCE-6258AA098B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533A9D0B-8582-4FA5-AB69-9A7A78FFD452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variation_ontology_list" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="1582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="1583">
   <si>
     <t>VariO:0001</t>
   </si>
@@ -4771,6 +4771,9 @@
   </si>
   <si>
     <t>hpo_mode_of_inheritance_term_definition</t>
+  </si>
+  <si>
+    <t>inheritance_filter</t>
   </si>
 </sst>
 </file>
@@ -5129,7 +5132,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5139,7 +5142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E496"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -12144,9 +12147,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -12167,6 +12170,9 @@
       <c r="C1" s="1" t="s">
         <v>1581</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>1582</v>
+      </c>
       <c r="E1" s="1" t="s">
         <v>1482</v>
       </c>
@@ -12186,6 +12192,9 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>1487</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.65">

</xml_diff>